<commit_message>
update on components and sim file
</commit_message>
<xml_diff>
--- a/Component_List.xlsx
+++ b/Component_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Optimus-Primary-Winding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7C4280-ECE2-4896-956A-BCD58A30AB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FB066D-0CF7-435E-AACA-EE00A53F7632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="11364" windowWidth="23256" windowHeight="13896" xr2:uid="{ABAF7D5C-48AB-41E3-A9CD-5B03435CF991}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABAF7D5C-48AB-41E3-A9CD-5B03435CF991}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Component</t>
   </si>
@@ -60,6 +60,89 @@
   </si>
   <si>
     <t>FERRITE CORE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Caps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- 1u x3 (25V for input x1)
+-1n x3
+-2n x1
+-330n(50V) x1
+-330p(150V) x1
+-47u or 68u (63V for output) x1</t>
+    </r>
+  </si>
+  <si>
+    <t>TL431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC3842 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resistor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-480R (min 2W) x1
+-0.05R (5W sense)x1
+-10k x5 (x1 %1 tolerance for controller)
+-1k x1
+-600k x1
+-182k x1 (%1 tolerance)
+-14.3k x1
+-22.2k x2
+-10R x1
+-100R x1
+-4.7k x1
+-5k x1</t>
+    </r>
+  </si>
+  <si>
+    <t>30V Zener</t>
+  </si>
+  <si>
+    <t>15V Zener (Depending on max switch voltage)</t>
+  </si>
+  <si>
+    <t>2N2222 x2</t>
   </si>
 </sst>
 </file>
@@ -67,9 +150,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +177,15 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,13 +249,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -607,15 +702,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E520E67-1D27-4A68-9886-D4EF86CBEAFA}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44.77734375" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="70.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
   </cols>
@@ -654,50 +749,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>

</xml_diff>

<commit_message>
Simulations and Design Decisions
</commit_message>
<xml_diff>
--- a/Component_List.xlsx
+++ b/Component_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Optimus-Primary-Winding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FB066D-0CF7-435E-AACA-EE00A53F7632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F925D8-F0DD-43B9-882F-5ACADC762B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABAF7D5C-48AB-41E3-A9CD-5B03435CF991}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Component</t>
   </si>
@@ -96,7 +96,85 @@
     <t>TL431</t>
   </si>
   <si>
-    <t xml:space="preserve">UC3842 </t>
+    <t>IC-4N25 OPTO 5300V TRANS.OUTPUT SMD6 LITEON</t>
+  </si>
+  <si>
+    <t>0,17620 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/optolar-ve-sensorler/optolar/transistor-cikisli-optokuplorler/4N25S-TA1/434368</t>
+  </si>
+  <si>
+    <t>4N25 Optocoupler</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/2n2222-transistor-bjt-npn-to-92</t>
+  </si>
+  <si>
+    <t>2N2222 Transistör BJT TO-92 - NPN 6V 0.8A</t>
+  </si>
+  <si>
+    <t>0,99 TL</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE ZENER 300mW 15V SOD323 </t>
+  </si>
+  <si>
+    <t>15V Zener (Voltage depends on Vds)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/zener-diyotlar/MM3Z15VT1G/625608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,03367 USD</t>
+  </si>
+  <si>
+    <t>DIODE ZENER 500mW 30V ±5% SOD123 SMT</t>
+  </si>
+  <si>
+    <t>30V Zener (For Linear Regulator)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/zener-diyotlar/MMSZ4713-VR100001/563477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,05405 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/entegre-devreler-ics/guc-entegreleri/voltage-reference-entegreleri/TL431AIDBZR/341981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,18929 USD</t>
+  </si>
+  <si>
+    <t>Precision Programmable Reference</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/entegre-devreler-ics/guc-entegreleri/dc-dc-voltaj-kontrolorleri/UC3843AD8TR/461759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC-3843 REG. CONTROLLER PWM CM SOIC8 </t>
+  </si>
+  <si>
+    <t>PWM Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,06870 USD </t>
+  </si>
+  <si>
+    <t>RES.SHUNT (6432) 2512 47m Ohms 1% 4W AUTO SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,80477 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/pasif-komponentler/direncler/hassas-ve-sont-direncler/VMS-R047-1-0-U/536795</t>
+  </si>
+  <si>
+    <t>47m Sense Resistor 4W</t>
   </si>
   <si>
     <r>
@@ -121,8 +199,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
--480R (min 2W) x1
--0.05R (5W sense)x1
+-480R (min 2W) x1 Kalsın şimdilik 1k seçeceğiz
+-0.05R (5W sense)x1 
 -10k x5 (x1 %1 tolerance for controller)
 -1k x1
 -600k x1
@@ -134,15 +212,6 @@
 -4.7k x1
 -5k x1</t>
     </r>
-  </si>
-  <si>
-    <t>30V Zener</t>
-  </si>
-  <si>
-    <t>15V Zener (Depending on max switch voltage)</t>
-  </si>
-  <si>
-    <t>2N2222 x2</t>
   </si>
 </sst>
 </file>
@@ -249,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -261,6 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -391,7 +461,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B831FA0-2FF9-4170-BC4D-1B3E0F7BB767}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B831FA0-2FF9-4170-BC4D-1B3E0F7BB767}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4DB572EA-B97E-43B7-8E61-6CC55990BA4F}" name="Component" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{03E7016A-1F49-4A13-8941-D150A9A2F6CF}" name="Price" dataDxfId="3"/>
@@ -700,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E520E67-1D27-4A68-9886-D4EF86CBEAFA}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,7 +830,7 @@
     </row>
     <row r="4" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -771,63 +841,144 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{B2B197F7-B723-4767-8FE3-BB13551641B6}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{7D50748C-81DF-4AF5-BE75-9E1FBF073886}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{6B657A83-BD45-407D-8C46-CCFAC6ABD1F2}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{931391FE-2493-4D41-9D9A-CB2AC8A2E7EF}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{ACB79ED0-7A44-4B9B-B9C2-1A4CDF9482D2}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{D1B8B35A-5104-41AC-84B4-59AE700C7DF8}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{BA19392D-52DE-438F-B1DF-611969A140A8}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{E8102777-57D3-4906-8ADE-02234FEDE441}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update on components and simulation
</commit_message>
<xml_diff>
--- a/Component_List.xlsx
+++ b/Component_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Optimus-Primary-Winding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E825D4-9F42-4306-8B75-9EEF590F1B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A969197-E772-4699-BCCE-7DA4F28BF42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABAF7D5C-48AB-41E3-A9CD-5B03435CF991}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Component</t>
   </si>
@@ -212,6 +212,42 @@
 -4.7k x1
 -5k x1</t>
     </r>
+  </si>
+  <si>
+    <t>MOSFET DIS.17A 55V N-CH TO252(DPAK) HEXFET SMT</t>
+  </si>
+  <si>
+    <t>55V 17A MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,41515 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/IRFR024NTRPBF/372863</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 10A 150V TO220AC THT</t>
+  </si>
+  <si>
+    <t>150V 10A Schottky Diode</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/schottky-diyotlar/MBR10150T000001/573568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,47311 USD</t>
+  </si>
+  <si>
+    <t>DIODE STAND. Single 1A 100V THT DO41</t>
+  </si>
+  <si>
+    <t>100V 1A Diode</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/genel-amacli-diyotlar/1N4002/735859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,02037 USD</t>
   </si>
 </sst>
 </file>
@@ -461,7 +497,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B831FA0-2FF9-4170-BC4D-1B3E0F7BB767}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B831FA0-2FF9-4170-BC4D-1B3E0F7BB767}" name="Table1" displayName="Table1" ref="A1:E15" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4DB572EA-B97E-43B7-8E61-6CC55990BA4F}" name="Component" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{03E7016A-1F49-4A13-8941-D150A9A2F6CF}" name="Price" dataDxfId="3"/>
@@ -770,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E520E67-1D27-4A68-9886-D4EF86CBEAFA}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,6 +999,57 @@
         <v>36</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -974,11 +1061,14 @@
     <hyperlink ref="C5" r:id="rId6" xr:uid="{D1B8B35A-5104-41AC-84B4-59AE700C7DF8}"/>
     <hyperlink ref="C6" r:id="rId7" xr:uid="{BA19392D-52DE-438F-B1DF-611969A140A8}"/>
     <hyperlink ref="C12" r:id="rId8" xr:uid="{E8102777-57D3-4906-8ADE-02234FEDE441}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{8B5D96BA-85FD-42CD-9C24-0643C8E1C474}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{6EA39D5E-79D6-4292-B14E-B73FDD19C9B0}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{FEA88C98-0AF0-4A23-AB2E-B86572892D5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updates on component list  simulation
</commit_message>
<xml_diff>
--- a/Component_List.xlsx
+++ b/Component_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Optimus-Primary-Winding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A969197-E772-4699-BCCE-7DA4F28BF42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2D9EE5-B475-44DE-8D4F-D71EEA44326B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABAF7D5C-48AB-41E3-A9CD-5B03435CF991}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Component</t>
   </si>
@@ -60,6 +60,159 @@
   </si>
   <si>
     <t>FERRITE CORE</t>
+  </si>
+  <si>
+    <t>TL431</t>
+  </si>
+  <si>
+    <t>IC-4N25 OPTO 5300V TRANS.OUTPUT SMD6 LITEON</t>
+  </si>
+  <si>
+    <t>0,17620 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/optolar-ve-sensorler/optolar/transistor-cikisli-optokuplorler/4N25S-TA1/434368</t>
+  </si>
+  <si>
+    <t>4N25 Optocoupler</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/2n2222-transistor-bjt-npn-to-92</t>
+  </si>
+  <si>
+    <t>2N2222 Transistör BJT TO-92 - NPN 6V 0.8A</t>
+  </si>
+  <si>
+    <t>0,99 TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE ZENER 300mW 15V SOD323 </t>
+  </si>
+  <si>
+    <t>15V Zener (Voltage depends on Vds)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/zener-diyotlar/MM3Z15VT1G/625608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,03367 USD</t>
+  </si>
+  <si>
+    <t>DIODE ZENER 500mW 30V ±5% SOD123 SMT</t>
+  </si>
+  <si>
+    <t>30V Zener (For Linear Regulator)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/zener-diyotlar/MMSZ4713-VR100001/563477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,05405 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/entegre-devreler-ics/guc-entegreleri/voltage-reference-entegreleri/TL431AIDBZR/341981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,18929 USD</t>
+  </si>
+  <si>
+    <t>Precision Programmable Reference</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/entegre-devreler-ics/guc-entegreleri/dc-dc-voltaj-kontrolorleri/UC3843AD8TR/461759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC-3843 REG. CONTROLLER PWM CM SOIC8 </t>
+  </si>
+  <si>
+    <t>PWM Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,06870 USD </t>
+  </si>
+  <si>
+    <t>MOSFET DIS.17A 55V N-CH TO252(DPAK) HEXFET SMT</t>
+  </si>
+  <si>
+    <t>55V 17A MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,41515 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/IRFR024NTRPBF/372863</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 10A 150V TO220AC THT</t>
+  </si>
+  <si>
+    <t>150V 10A Schottky Diode</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/schottky-diyotlar/MBR10150T000001/573568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,47311 USD</t>
+  </si>
+  <si>
+    <t>DIODE STAND. Single 1A 100V THT DO41</t>
+  </si>
+  <si>
+    <t>100V 1A Diode</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/genel-amacli-diyotlar/1N4002/735859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0,02037 USD</t>
+  </si>
+  <si>
+    <t>RES.SHUNT (6432) 2512 150m Ohms 1% 4W AUTO SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		0,80546 USD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/pasif-komponentler/direncler/hassas-ve-sont-direncler/VMS-R150-1-0-U/536802</t>
+  </si>
+  <si>
+    <t>150m Sense Resistor 4W</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resistor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-2.2k 1W x2
+-100R 1W x1
+-47R 1W x1
+-150m (4W) x3 (aşağıda yazdım)
+-10R x1
+-1k x1
+-22k x3
+-4.7k x2
+-10k x3
+-100k x1 + 82k x1 (%1 olursa iyi olur)
+-820k x1</t>
+    </r>
   </si>
   <si>
     <r>
@@ -84,170 +237,30 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-- 1u x3 (25V for input x1)
--1n x3
--2n x1
--330n(50V) x1
--330p(150V) x1
--47u or 68u (63V for output) x1</t>
+-1u 25V x1
+-220n 63V x1
+-1uF x2
+-100pF x1
+-4.7nF 63V x1
+-470pF x1
+-2.2nF x1
+-1nF x1
+-270pF 1000V x1 (150V yok mecbur 1000)
+-47uF 100V x1
+</t>
     </r>
   </si>
   <si>
-    <t>TL431</t>
-  </si>
-  <si>
-    <t>IC-4N25 OPTO 5300V TRANS.OUTPUT SMD6 LITEON</t>
-  </si>
-  <si>
-    <t>0,17620 USD</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/optolar-ve-sensorler/optolar/transistor-cikisli-optokuplorler/4N25S-TA1/434368</t>
-  </si>
-  <si>
-    <t>4N25 Optocoupler</t>
-  </si>
-  <si>
-    <t>https://www.direnc.net/2n2222-transistor-bjt-npn-to-92</t>
-  </si>
-  <si>
-    <t>2N2222 Transistör BJT TO-92 - NPN 6V 0.8A</t>
-  </si>
-  <si>
-    <t>0,99 TL</t>
-  </si>
-  <si>
-    <t>Fuse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE ZENER 300mW 15V SOD323 </t>
-  </si>
-  <si>
-    <t>15V Zener (Voltage depends on Vds)</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/zener-diyotlar/MM3Z15VT1G/625608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,03367 USD</t>
-  </si>
-  <si>
-    <t>DIODE ZENER 500mW 30V ±5% SOD123 SMT</t>
-  </si>
-  <si>
-    <t>30V Zener (For Linear Regulator)</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/zener-diyotlar/MMSZ4713-VR100001/563477</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,05405 USD</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/entegre-devreler-ics/guc-entegreleri/voltage-reference-entegreleri/TL431AIDBZR/341981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,18929 USD</t>
-  </si>
-  <si>
-    <t>Precision Programmable Reference</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/entegre-devreler-ics/guc-entegreleri/dc-dc-voltaj-kontrolorleri/UC3843AD8TR/461759</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC-3843 REG. CONTROLLER PWM CM SOIC8 </t>
-  </si>
-  <si>
-    <t>PWM Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,06870 USD </t>
-  </si>
-  <si>
-    <t>RES.SHUNT (6432) 2512 47m Ohms 1% 4W AUTO SMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,80477 USD</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/pasif-komponentler/direncler/hassas-ve-sont-direncler/VMS-R047-1-0-U/536795</t>
-  </si>
-  <si>
-    <t>47m Sense Resistor 4W</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="162"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Resistor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="162"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--480R (min 2W) x1 Kalsın şimdilik 1k seçeceğiz
--0.05R (5W sense)x1 aşağıda yazdım
--10k x5 (x1 %1 tolerance for controller)
--1k x1
--600k x1
--182k x1 (%1 tolerance172k +1k olabilir)
--14.3k x1
--22.2k x2
--10R x1
--100R x1
--4.7k x1
--5k x1</t>
-    </r>
-  </si>
-  <si>
-    <t>MOSFET DIS.17A 55V N-CH TO252(DPAK) HEXFET SMT</t>
-  </si>
-  <si>
-    <t>55V 17A MOSFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,41515 USD</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/IRFR024NTRPBF/372863</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 10A 150V TO220AC THT</t>
-  </si>
-  <si>
-    <t>150V 10A Schottky Diode</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/schottky-diyotlar/MBR10150T000001/573568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,47311 USD</t>
-  </si>
-  <si>
-    <t>DIODE STAND. Single 1A 100V THT DO41</t>
-  </si>
-  <si>
-    <t>100V 1A Diode</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/guc-yari-iletkenleri/diyotlar-modul-diyotlar-ve-dogrultucular/genel-amacli-diyotlar/1N4002/735859</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	0,02037 USD</t>
+    <t>25A Fuse</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/25a-ufak-cam-sigorta-20mm</t>
+  </si>
+  <si>
+    <t>0,54 TL</t>
+  </si>
+  <si>
+    <t>25A 5x20mm Cam Sigorta</t>
   </si>
 </sst>
 </file>
@@ -809,7 +822,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,18 +868,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -875,81 +888,81 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -958,96 +971,104 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D12" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1060,15 +1081,16 @@
     <hyperlink ref="C7" r:id="rId5" xr:uid="{ACB79ED0-7A44-4B9B-B9C2-1A4CDF9482D2}"/>
     <hyperlink ref="C5" r:id="rId6" xr:uid="{D1B8B35A-5104-41AC-84B4-59AE700C7DF8}"/>
     <hyperlink ref="C6" r:id="rId7" xr:uid="{BA19392D-52DE-438F-B1DF-611969A140A8}"/>
-    <hyperlink ref="C12" r:id="rId8" xr:uid="{E8102777-57D3-4906-8ADE-02234FEDE441}"/>
-    <hyperlink ref="C13" r:id="rId9" xr:uid="{8B5D96BA-85FD-42CD-9C24-0643C8E1C474}"/>
-    <hyperlink ref="C14" r:id="rId10" xr:uid="{6EA39D5E-79D6-4292-B14E-B73FDD19C9B0}"/>
-    <hyperlink ref="C15" r:id="rId11" xr:uid="{FEA88C98-0AF0-4A23-AB2E-B86572892D5C}"/>
+    <hyperlink ref="C13" r:id="rId8" xr:uid="{8B5D96BA-85FD-42CD-9C24-0643C8E1C474}"/>
+    <hyperlink ref="C14" r:id="rId9" xr:uid="{6EA39D5E-79D6-4292-B14E-B73FDD19C9B0}"/>
+    <hyperlink ref="C15" r:id="rId10" xr:uid="{FEA88C98-0AF0-4A23-AB2E-B86572892D5C}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{1FF546A1-4934-409C-B256-115BFD2524FA}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{6AEEFA12-132A-4BC1-9150-B762C964078C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Presentation for simulations and thermal design
</commit_message>
<xml_diff>
--- a/Component_List.xlsx
+++ b/Component_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Optimus-Primary-Winding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D665B9-D65C-41C5-9075-C21CE6543D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E64B29-176B-4F97-8F68-A691FD50BE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABAF7D5C-48AB-41E3-A9CD-5B03435CF991}"/>
   </bookViews>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E520E67-1D27-4A68-9886-D4EF86CBEAFA}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>